<commit_message>
revisian kpi dari bu vega, redesain
</commit_message>
<xml_diff>
--- a/public/import/Job_Position_Template.xlsx
+++ b/public/import/Job_Position_Template.xlsx
@@ -1,36 +1,63 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS-A4\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\busdev-pc\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA1D258-6D51-43AA-9582-651D3CE86BFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" forceFullCalc="1"/>
+  <calcPr calcId="191029" forceFullCalc="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>job_position</t>
   </si>
   <si>
-    <t>BUSINESS process staff</t>
+    <t>Recruitment Officer</t>
+  </si>
+  <si>
+    <t>Personnel Officer</t>
+  </si>
+  <si>
+    <t>General Affair Officer</t>
+  </si>
+  <si>
+    <t>Trainner Officer</t>
+  </si>
+  <si>
+    <t>Human Resource Supervisor</t>
+  </si>
+  <si>
+    <t>Legal Supervisor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -363,11 +390,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F8" sqref="F8:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -382,6 +409,31 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>